<commit_message>
update semua yang saya ubah
</commit_message>
<xml_diff>
--- a/MonitoringSystem/wwwroot/data/cs/plan/cs_plan_template.xlsx
+++ b/MonitoringSystem/wwwroot/data/cs/plan/cs_plan_template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\KP\repos\testXLS\testXLS\wwwroot\data\cs\plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mghaz\Magang Panasonic\WebMon_8.5_Pub - Revisi Pak Awan\MonitoringSystem\wwwroot\data\cs\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60A2EC8-3640-4374-ABFE-0D1401C6E9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="167">
-  <si>
-    <t>Tanggal</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="166">
   <si>
     <t>CS-YN5TKJ</t>
   </si>
@@ -530,7 +528,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -845,11 +843,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF211"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AF210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="Q215" sqref="Q215"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -858,101 +856,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D1" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E1" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F1" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G1" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H1" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I1" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J1" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K1" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L1" s="1">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="M1" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="N1" s="1">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="O1" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="P1" s="1">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Q1" s="1">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R1" s="1">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="S1" s="1">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="T1" s="1">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="U1" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="V1" s="1">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="W1" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="X1" s="1">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="Y1" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="Z1" s="1">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="AA1" s="1">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="AB1" s="1">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="AC1" s="1">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="AD1" s="1">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="AE1" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AF1" s="1">
-        <v>31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
@@ -16735,7 +16733,7 @@
     </row>
     <row r="163" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>162</v>
+        <v>104</v>
       </c>
       <c r="B163" s="1">
         <v>0</v>
@@ -21047,7 +21045,7 @@
     </row>
     <row r="207" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="B207" s="1">
         <v>0</v>
@@ -21434,104 +21432,6 @@
         <v>0</v>
       </c>
       <c r="AF210" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="211" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A211" t="s">
-        <v>166</v>
-      </c>
-      <c r="B211" s="1">
-        <v>0</v>
-      </c>
-      <c r="C211" s="1">
-        <v>0</v>
-      </c>
-      <c r="D211" s="1">
-        <v>0</v>
-      </c>
-      <c r="E211" s="1">
-        <v>0</v>
-      </c>
-      <c r="F211" s="1">
-        <v>0</v>
-      </c>
-      <c r="G211" s="1">
-        <v>0</v>
-      </c>
-      <c r="H211" s="1">
-        <v>0</v>
-      </c>
-      <c r="I211" s="1">
-        <v>0</v>
-      </c>
-      <c r="J211" s="1">
-        <v>0</v>
-      </c>
-      <c r="K211" s="1">
-        <v>0</v>
-      </c>
-      <c r="L211" s="1">
-        <v>0</v>
-      </c>
-      <c r="M211" s="1">
-        <v>0</v>
-      </c>
-      <c r="N211" s="1">
-        <v>0</v>
-      </c>
-      <c r="O211" s="1">
-        <v>0</v>
-      </c>
-      <c r="P211" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q211" s="1">
-        <v>0</v>
-      </c>
-      <c r="R211" s="1">
-        <v>0</v>
-      </c>
-      <c r="S211" s="1">
-        <v>0</v>
-      </c>
-      <c r="T211" s="1">
-        <v>0</v>
-      </c>
-      <c r="U211" s="1">
-        <v>0</v>
-      </c>
-      <c r="V211" s="1">
-        <v>0</v>
-      </c>
-      <c r="W211" s="1">
-        <v>0</v>
-      </c>
-      <c r="X211" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y211" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z211" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA211" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB211" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC211" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD211" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE211" s="1">
-        <v>0</v>
-      </c>
-      <c r="AF211" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>